<commit_message>
fim do desafio outlook python minha resolucao
</commit_message>
<xml_diff>
--- a/023-integracaoPythonEmail/02-explicacaoDoDesafio/Enviar E-mails.xlsx
+++ b/023-integracaoPythonEmail/02-explicacaoDoDesafio/Enviar E-mails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jharbes\Documents\GitHub\hashtagPython\023-integracaoPythonEmail\02-explicacaoDoDesafio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF25E99-10E8-4B1E-BCF7-5EA79B7C971E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9909036A-C515-487A-85BC-9F73D6BA13A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F493D48C-57DD-448B-A29F-0870F5FA714B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Gerente</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>jharbes@hotmail.com</t>
+  </si>
+  <si>
+    <t>jharbes@icloud.com</t>
+  </si>
+  <si>
+    <t>jorge.harbes@technipfmc.com</t>
+  </si>
+  <si>
+    <t>jorgenamiharbes@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -453,7 +462,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +498,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -500,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -511,7 +520,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -533,7 +542,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -544,7 +553,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>

</xml_diff>